<commit_message>
Some Changes related to base logic.
</commit_message>
<xml_diff>
--- a/Test_Data/TestData.xlsx
+++ b/Test_Data/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\final\rest-api-testing-using-RestAssured-master\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\finalOne\apiAutomation\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25356" yWindow="108" windowWidth="14808" windowHeight="6576"/>
+    <workbookView xWindow="26448" yWindow="108" windowWidth="14808" windowHeight="6576"/>
   </bookViews>
   <sheets>
     <sheet name="Booking" sheetId="1" r:id="rId1"/>
@@ -135,34 +135,34 @@
     <t>2019-04-21</t>
   </si>
   <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>712</t>
+  </si>
+  <si>
+    <t>2015-05-04</t>
+  </si>
+  <si>
+    <t>2019-04-02</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>2018-01-01</t>
+  </si>
+  <si>
+    <t>2019-01-01</t>
+  </si>
+  <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Marie</t>
-  </si>
-  <si>
-    <t>712</t>
-  </si>
-  <si>
-    <t>2015-05-04</t>
-  </si>
-  <si>
-    <t>2019-04-02</t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>2018-01-01</t>
-  </si>
-  <si>
-    <t>2019-01-01</t>
   </si>
 </sst>
 </file>
@@ -625,7 +625,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,22 +691,22 @@
         <v>12</v>
       </c>
       <c r="D2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>45</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>16</v>
@@ -720,7 +720,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>34</v>
@@ -755,7 +755,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>13</v>
@@ -790,28 +790,28 @@
         <v>25</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>23</v>
       </c>
       <c r="H5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="12" t="s">

</xml_diff>